<commit_message>
Ajustei a planilha de Riscos, e alguns layouts
</commit_message>
<xml_diff>
--- a/Riscos do projeto.xlsx
+++ b/Riscos do projeto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\OneDrive\Sptech\Algoritmo\ENTREGÁVEIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gfran\Desktop\HardwareLife\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>